<commit_message>
version 1 of herb synonyms
There are two csv, if there is exact herb found, the synonyms are added into synonyms_herb_exact.csv; else the synonyms of similar herb are added into synonyms_herb_similar.csv
</commit_message>
<xml_diff>
--- a/demo.xlsx
+++ b/demo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mycuhk-my.sharepoint.com/personal/1155143802_link_cuhk_edu_hk/Documents/GitHub/Pharmacy Automation - Breast Cancer HDI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{9E9A464B-D117-9348-ACC9-A1CAF201185F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B8B5D538-8D68-DE48-97BF-B49698AD1473}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{9E9A464B-D117-9348-ACC9-A1CAF201185F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AEA48733-66D9-5049-9BF3-8DF501A96606}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="10200" windowWidth="15120" windowHeight="9440" xr2:uid="{592CA08D-34E1-B340-AB48-B4EDA4297DF2}"/>
+    <workbookView xWindow="15120" yWindow="10200" windowWidth="15120" windowHeight="9440" xr2:uid="{592CA08D-34E1-B340-AB48-B4EDA4297DF2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,32 +36,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>Chemotherapy</t>
+    <t>三七</t>
   </si>
   <si>
-    <t>Adriamycin</t>
+    <t>丝瓜络</t>
   </si>
   <si>
-    <t>Epirubicin</t>
+    <t>三棱</t>
+  </si>
+  <si>
+    <t>丹参</t>
+  </si>
+  <si>
+    <t>丹皮</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -88,14 +86,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -106,6 +114,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -405,30 +417,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A508191-8C33-2D4B-93C8-FF9624188AAA}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A1:A5">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>